<commit_message>
documentos preenchidos, falta cenario de testes
</commit_message>
<xml_diff>
--- a/lista_verificacao_individual_Pedro_Magaieski.xlsx
+++ b/lista_verificacao_individual_Pedro_Magaieski.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\46140459877\Documents\Saep\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{474F68FB-21A7-473D-8AB2-49D93F83FD32}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05501514-0B47-444E-BAC0-E89C72DB103D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="20370" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -782,6 +782,63 @@
     <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -791,65 +848,8 @@
     <xf numFmtId="0" fontId="6" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1248,8 +1248,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J62"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A28" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="J33" sqref="J33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1267,26 +1267,26 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="40" t="s">
+      <c r="A1" s="25" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="41"/>
-      <c r="C1" s="41"/>
-      <c r="D1" s="41"/>
-      <c r="E1" s="41"/>
-      <c r="F1" s="41"/>
-      <c r="G1" s="41"/>
-      <c r="H1" s="41"/>
-      <c r="I1" s="41"/>
+      <c r="B1" s="26"/>
+      <c r="C1" s="26"/>
+      <c r="D1" s="26"/>
+      <c r="E1" s="26"/>
+      <c r="F1" s="26"/>
+      <c r="G1" s="26"/>
+      <c r="H1" s="26"/>
+      <c r="I1" s="26"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="42" t="s">
+      <c r="B3" s="33" t="s">
         <v>124</v>
       </c>
-      <c r="C3" s="43"/>
+      <c r="C3" s="34"/>
       <c r="D3" s="10" t="s">
         <v>125</v>
       </c>
@@ -1300,10 +1300,10 @@
       <c r="A4" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="44" t="s">
+      <c r="B4" s="35" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="45"/>
+      <c r="C4" s="36"/>
       <c r="D4" s="10" t="s">
         <v>126</v>
       </c>
@@ -1338,15 +1338,15 @@
       <c r="A6" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="B6" s="44" t="s">
+      <c r="B6" s="35" t="s">
         <v>10</v>
       </c>
-      <c r="C6" s="46"/>
-      <c r="D6" s="45"/>
-      <c r="E6" s="47" t="s">
+      <c r="C6" s="37"/>
+      <c r="D6" s="36"/>
+      <c r="E6" s="38" t="s">
         <v>127</v>
       </c>
-      <c r="F6" s="47"/>
+      <c r="F6" s="38"/>
       <c r="G6" s="17"/>
       <c r="H6" s="17"/>
       <c r="I6" s="17"/>
@@ -1384,10 +1384,10 @@
       </c>
     </row>
     <row r="9" spans="1:10" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="37" t="s">
+      <c r="A9" s="30" t="s">
         <v>20</v>
       </c>
-      <c r="B9" s="37" t="s">
+      <c r="B9" s="30" t="s">
         <v>21</v>
       </c>
       <c r="C9" s="7" t="s">
@@ -1410,8 +1410,8 @@
       </c>
     </row>
     <row r="10" spans="1:10" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="38"/>
-      <c r="B10" s="38"/>
+      <c r="A10" s="31"/>
+      <c r="B10" s="31"/>
       <c r="C10" s="3" t="s">
         <v>26</v>
       </c>
@@ -1432,12 +1432,12 @@
       </c>
     </row>
     <row r="11" spans="1:10" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="38"/>
-      <c r="B11" s="38"/>
-      <c r="C11" s="37" t="s">
+      <c r="A11" s="31"/>
+      <c r="B11" s="31"/>
+      <c r="C11" s="30" t="s">
         <v>30</v>
       </c>
-      <c r="D11" s="34" t="s">
+      <c r="D11" s="27" t="s">
         <v>31</v>
       </c>
       <c r="E11" s="7" t="s">
@@ -1451,10 +1451,10 @@
       <c r="I11" s="8"/>
     </row>
     <row r="12" spans="1:10" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="38"/>
-      <c r="B12" s="38"/>
-      <c r="C12" s="38"/>
-      <c r="D12" s="35"/>
+      <c r="A12" s="31"/>
+      <c r="B12" s="31"/>
+      <c r="C12" s="31"/>
+      <c r="D12" s="28"/>
       <c r="E12" s="7" t="s">
         <v>34</v>
       </c>
@@ -1466,10 +1466,10 @@
       <c r="I12" s="8"/>
     </row>
     <row r="13" spans="1:10" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="38"/>
-      <c r="B13" s="38"/>
-      <c r="C13" s="39"/>
-      <c r="D13" s="36"/>
+      <c r="A13" s="31"/>
+      <c r="B13" s="31"/>
+      <c r="C13" s="32"/>
+      <c r="D13" s="29"/>
       <c r="E13" s="7" t="s">
         <v>36</v>
       </c>
@@ -1481,12 +1481,12 @@
       <c r="I13" s="8"/>
     </row>
     <row r="14" spans="1:10" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="38"/>
-      <c r="B14" s="38"/>
-      <c r="C14" s="30" t="s">
+      <c r="A14" s="31"/>
+      <c r="B14" s="31"/>
+      <c r="C14" s="39" t="s">
         <v>38</v>
       </c>
-      <c r="D14" s="28" t="s">
+      <c r="D14" s="42" t="s">
         <v>39</v>
       </c>
       <c r="E14" s="3" t="s">
@@ -1503,10 +1503,10 @@
       </c>
     </row>
     <row r="15" spans="1:10" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="38"/>
-      <c r="B15" s="39"/>
-      <c r="C15" s="31"/>
-      <c r="D15" s="29"/>
+      <c r="A15" s="31"/>
+      <c r="B15" s="32"/>
+      <c r="C15" s="41"/>
+      <c r="D15" s="43"/>
       <c r="E15" s="3" t="s">
         <v>42</v>
       </c>
@@ -1518,14 +1518,14 @@
       <c r="I15" s="4"/>
     </row>
     <row r="16" spans="1:10" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="38"/>
-      <c r="B16" s="37" t="s">
+      <c r="A16" s="31"/>
+      <c r="B16" s="30" t="s">
         <v>44</v>
       </c>
-      <c r="C16" s="37" t="s">
+      <c r="C16" s="30" t="s">
         <v>45</v>
       </c>
-      <c r="D16" s="34" t="s">
+      <c r="D16" s="27" t="s">
         <v>46</v>
       </c>
       <c r="E16" s="7" t="s">
@@ -1539,10 +1539,10 @@
       <c r="I16" s="8"/>
     </row>
     <row r="17" spans="1:10" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="38"/>
-      <c r="B17" s="38"/>
-      <c r="C17" s="38"/>
-      <c r="D17" s="35"/>
+      <c r="A17" s="31"/>
+      <c r="B17" s="31"/>
+      <c r="C17" s="31"/>
+      <c r="D17" s="28"/>
       <c r="E17" s="7" t="s">
         <v>49</v>
       </c>
@@ -1554,10 +1554,10 @@
       <c r="I17" s="8"/>
     </row>
     <row r="18" spans="1:10" ht="45" x14ac:dyDescent="0.25">
-      <c r="A18" s="38"/>
-      <c r="B18" s="38"/>
-      <c r="C18" s="38"/>
-      <c r="D18" s="35"/>
+      <c r="A18" s="31"/>
+      <c r="B18" s="31"/>
+      <c r="C18" s="31"/>
+      <c r="D18" s="28"/>
       <c r="E18" s="7" t="s">
         <v>51</v>
       </c>
@@ -1572,10 +1572,10 @@
       </c>
     </row>
     <row r="19" spans="1:10" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="38"/>
-      <c r="B19" s="38"/>
-      <c r="C19" s="38"/>
-      <c r="D19" s="35"/>
+      <c r="A19" s="31"/>
+      <c r="B19" s="31"/>
+      <c r="C19" s="31"/>
+      <c r="D19" s="28"/>
       <c r="E19" s="7" t="s">
         <v>53</v>
       </c>
@@ -1587,10 +1587,10 @@
       <c r="I19" s="8"/>
     </row>
     <row r="20" spans="1:10" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="38"/>
-      <c r="B20" s="38"/>
-      <c r="C20" s="38"/>
-      <c r="D20" s="35"/>
+      <c r="A20" s="31"/>
+      <c r="B20" s="31"/>
+      <c r="C20" s="31"/>
+      <c r="D20" s="28"/>
       <c r="E20" s="7" t="s">
         <v>55</v>
       </c>
@@ -1602,10 +1602,10 @@
       <c r="I20" s="8"/>
     </row>
     <row r="21" spans="1:10" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="38"/>
-      <c r="B21" s="38"/>
-      <c r="C21" s="38"/>
-      <c r="D21" s="35"/>
+      <c r="A21" s="31"/>
+      <c r="B21" s="31"/>
+      <c r="C21" s="31"/>
+      <c r="D21" s="28"/>
       <c r="E21" s="7" t="s">
         <v>57</v>
       </c>
@@ -1620,10 +1620,10 @@
       </c>
     </row>
     <row r="22" spans="1:10" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="38"/>
-      <c r="B22" s="38"/>
-      <c r="C22" s="38"/>
-      <c r="D22" s="35"/>
+      <c r="A22" s="31"/>
+      <c r="B22" s="31"/>
+      <c r="C22" s="31"/>
+      <c r="D22" s="28"/>
       <c r="E22" s="7" t="s">
         <v>59</v>
       </c>
@@ -1635,10 +1635,10 @@
       <c r="I22" s="8"/>
     </row>
     <row r="23" spans="1:10" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="38"/>
-      <c r="B23" s="38"/>
-      <c r="C23" s="38"/>
-      <c r="D23" s="35"/>
+      <c r="A23" s="31"/>
+      <c r="B23" s="31"/>
+      <c r="C23" s="31"/>
+      <c r="D23" s="28"/>
       <c r="E23" s="7" t="s">
         <v>61</v>
       </c>
@@ -1650,10 +1650,10 @@
       <c r="I23" s="8"/>
     </row>
     <row r="24" spans="1:10" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="38"/>
-      <c r="B24" s="38"/>
-      <c r="C24" s="38"/>
-      <c r="D24" s="35"/>
+      <c r="A24" s="31"/>
+      <c r="B24" s="31"/>
+      <c r="C24" s="31"/>
+      <c r="D24" s="28"/>
       <c r="E24" s="7" t="s">
         <v>63</v>
       </c>
@@ -1665,10 +1665,10 @@
       <c r="I24" s="8"/>
     </row>
     <row r="25" spans="1:10" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="38"/>
-      <c r="B25" s="38"/>
-      <c r="C25" s="38"/>
-      <c r="D25" s="35"/>
+      <c r="A25" s="31"/>
+      <c r="B25" s="31"/>
+      <c r="C25" s="31"/>
+      <c r="D25" s="28"/>
       <c r="E25" s="7" t="s">
         <v>65</v>
       </c>
@@ -1680,10 +1680,10 @@
       <c r="I25" s="8"/>
     </row>
     <row r="26" spans="1:10" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="38"/>
-      <c r="B26" s="38"/>
-      <c r="C26" s="38"/>
-      <c r="D26" s="35"/>
+      <c r="A26" s="31"/>
+      <c r="B26" s="31"/>
+      <c r="C26" s="31"/>
+      <c r="D26" s="28"/>
       <c r="E26" s="7" t="s">
         <v>66</v>
       </c>
@@ -1695,10 +1695,10 @@
       <c r="I26" s="8"/>
     </row>
     <row r="27" spans="1:10" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="38"/>
-      <c r="B27" s="38"/>
-      <c r="C27" s="38"/>
-      <c r="D27" s="35"/>
+      <c r="A27" s="31"/>
+      <c r="B27" s="31"/>
+      <c r="C27" s="31"/>
+      <c r="D27" s="28"/>
       <c r="E27" s="7" t="s">
         <v>67</v>
       </c>
@@ -1710,10 +1710,10 @@
       <c r="I27" s="8"/>
     </row>
     <row r="28" spans="1:10" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="38"/>
-      <c r="B28" s="38"/>
-      <c r="C28" s="38"/>
-      <c r="D28" s="35"/>
+      <c r="A28" s="31"/>
+      <c r="B28" s="31"/>
+      <c r="C28" s="31"/>
+      <c r="D28" s="28"/>
       <c r="E28" s="7" t="s">
         <v>68</v>
       </c>
@@ -1725,10 +1725,10 @@
       <c r="I28" s="8"/>
     </row>
     <row r="29" spans="1:10" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="38"/>
-      <c r="B29" s="38"/>
-      <c r="C29" s="38"/>
-      <c r="D29" s="35"/>
+      <c r="A29" s="31"/>
+      <c r="B29" s="31"/>
+      <c r="C29" s="31"/>
+      <c r="D29" s="28"/>
       <c r="E29" s="7" t="s">
         <v>69</v>
       </c>
@@ -1740,10 +1740,10 @@
       <c r="I29" s="8"/>
     </row>
     <row r="30" spans="1:10" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="38"/>
-      <c r="B30" s="38"/>
-      <c r="C30" s="38"/>
-      <c r="D30" s="35"/>
+      <c r="A30" s="31"/>
+      <c r="B30" s="31"/>
+      <c r="C30" s="31"/>
+      <c r="D30" s="28"/>
       <c r="E30" s="7" t="s">
         <v>71</v>
       </c>
@@ -1755,10 +1755,10 @@
       <c r="I30" s="8"/>
     </row>
     <row r="31" spans="1:10" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="38"/>
-      <c r="B31" s="38"/>
-      <c r="C31" s="38"/>
-      <c r="D31" s="35"/>
+      <c r="A31" s="31"/>
+      <c r="B31" s="31"/>
+      <c r="C31" s="31"/>
+      <c r="D31" s="28"/>
       <c r="E31" s="7" t="s">
         <v>73</v>
       </c>
@@ -1771,10 +1771,10 @@
       <c r="J31" s="11"/>
     </row>
     <row r="32" spans="1:10" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="38"/>
-      <c r="B32" s="38"/>
-      <c r="C32" s="38"/>
-      <c r="D32" s="35"/>
+      <c r="A32" s="31"/>
+      <c r="B32" s="31"/>
+      <c r="C32" s="31"/>
+      <c r="D32" s="28"/>
       <c r="E32" s="7" t="s">
         <v>75</v>
       </c>
@@ -1786,10 +1786,10 @@
       <c r="I32" s="8"/>
     </row>
     <row r="33" spans="1:10" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="38"/>
-      <c r="B33" s="38"/>
-      <c r="C33" s="38"/>
-      <c r="D33" s="35"/>
+      <c r="A33" s="31"/>
+      <c r="B33" s="31"/>
+      <c r="C33" s="31"/>
+      <c r="D33" s="28"/>
       <c r="E33" s="7" t="s">
         <v>77</v>
       </c>
@@ -1801,10 +1801,10 @@
       <c r="I33" s="8"/>
     </row>
     <row r="34" spans="1:10" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="39"/>
-      <c r="B34" s="39"/>
-      <c r="C34" s="39"/>
-      <c r="D34" s="36"/>
+      <c r="A34" s="32"/>
+      <c r="B34" s="32"/>
+      <c r="C34" s="32"/>
+      <c r="D34" s="29"/>
       <c r="E34" s="7" t="s">
         <v>79</v>
       </c>
@@ -1819,16 +1819,16 @@
       </c>
     </row>
     <row r="35" spans="1:10" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="30" t="s">
+      <c r="A35" s="39" t="s">
         <v>81</v>
       </c>
-      <c r="B35" s="30" t="s">
+      <c r="B35" s="39" t="s">
         <v>82</v>
       </c>
-      <c r="C35" s="30" t="s">
+      <c r="C35" s="39" t="s">
         <v>83</v>
       </c>
-      <c r="D35" s="28" t="s">
+      <c r="D35" s="42" t="s">
         <v>84</v>
       </c>
       <c r="E35" s="3" t="s">
@@ -1838,17 +1838,17 @@
         <v>86</v>
       </c>
       <c r="G35" s="1"/>
-      <c r="H35" s="1"/>
+      <c r="H35" s="24"/>
       <c r="I35" s="4"/>
-      <c r="J35" s="25" t="s">
+      <c r="J35" s="44" t="s">
         <v>122</v>
       </c>
     </row>
     <row r="36" spans="1:10" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="33"/>
-      <c r="B36" s="33"/>
-      <c r="C36" s="31"/>
-      <c r="D36" s="29"/>
+      <c r="A36" s="40"/>
+      <c r="B36" s="40"/>
+      <c r="C36" s="41"/>
+      <c r="D36" s="43"/>
       <c r="E36" s="3" t="s">
         <v>87</v>
       </c>
@@ -1856,13 +1856,13 @@
         <v>88</v>
       </c>
       <c r="G36" s="1"/>
-      <c r="H36" s="1"/>
+      <c r="H36" s="24"/>
       <c r="I36" s="4"/>
-      <c r="J36" s="26"/>
+      <c r="J36" s="45"/>
     </row>
     <row r="37" spans="1:10" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="33"/>
-      <c r="B37" s="31"/>
+      <c r="A37" s="40"/>
+      <c r="B37" s="41"/>
       <c r="C37" s="7" t="s">
         <v>89</v>
       </c>
@@ -1876,19 +1876,19 @@
         <v>92</v>
       </c>
       <c r="G37" s="9"/>
-      <c r="H37" s="9"/>
+      <c r="H37" s="24"/>
       <c r="I37" s="8"/>
-      <c r="J37" s="26"/>
+      <c r="J37" s="45"/>
     </row>
     <row r="38" spans="1:10" ht="45" x14ac:dyDescent="0.25">
-      <c r="A38" s="33"/>
-      <c r="B38" s="30" t="s">
+      <c r="A38" s="40"/>
+      <c r="B38" s="39" t="s">
         <v>93</v>
       </c>
-      <c r="C38" s="30" t="s">
+      <c r="C38" s="39" t="s">
         <v>94</v>
       </c>
-      <c r="D38" s="28" t="s">
+      <c r="D38" s="42" t="s">
         <v>95</v>
       </c>
       <c r="E38" s="3" t="s">
@@ -1900,13 +1900,13 @@
       <c r="G38" s="23"/>
       <c r="H38" s="1"/>
       <c r="I38" s="4"/>
-      <c r="J38" s="26"/>
+      <c r="J38" s="45"/>
     </row>
     <row r="39" spans="1:10" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="33"/>
-      <c r="B39" s="33"/>
-      <c r="C39" s="33"/>
-      <c r="D39" s="32"/>
+      <c r="A39" s="40"/>
+      <c r="B39" s="40"/>
+      <c r="C39" s="40"/>
+      <c r="D39" s="47"/>
       <c r="E39" s="3" t="s">
         <v>98</v>
       </c>
@@ -1916,13 +1916,13 @@
       <c r="G39" s="23"/>
       <c r="H39" s="1"/>
       <c r="I39" s="4"/>
-      <c r="J39" s="26"/>
+      <c r="J39" s="45"/>
     </row>
     <row r="40" spans="1:10" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="33"/>
-      <c r="B40" s="31"/>
-      <c r="C40" s="31"/>
-      <c r="D40" s="29"/>
+      <c r="A40" s="40"/>
+      <c r="B40" s="41"/>
+      <c r="C40" s="41"/>
+      <c r="D40" s="43"/>
       <c r="E40" s="3" t="s">
         <v>100</v>
       </c>
@@ -1932,10 +1932,10 @@
       <c r="G40" s="23"/>
       <c r="H40" s="1"/>
       <c r="I40" s="4"/>
-      <c r="J40" s="26"/>
+      <c r="J40" s="45"/>
     </row>
     <row r="41" spans="1:10" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="33"/>
+      <c r="A41" s="40"/>
       <c r="B41" s="7" t="s">
         <v>102</v>
       </c>
@@ -1954,10 +1954,10 @@
       <c r="G41" s="23"/>
       <c r="H41" s="9"/>
       <c r="I41" s="8"/>
-      <c r="J41" s="26"/>
+      <c r="J41" s="45"/>
     </row>
     <row r="42" spans="1:10" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="31"/>
+      <c r="A42" s="41"/>
       <c r="B42" s="3" t="s">
         <v>107</v>
       </c>
@@ -1976,7 +1976,7 @@
       <c r="G42" s="23"/>
       <c r="H42" s="1"/>
       <c r="I42" s="4"/>
-      <c r="J42" s="27"/>
+      <c r="J42" s="46"/>
     </row>
     <row r="43" spans="1:10" x14ac:dyDescent="0.25">
       <c r="D43" s="13"/>
@@ -2040,13 +2040,11 @@
     </row>
   </sheetData>
   <mergeCells count="22">
-    <mergeCell ref="A1:I1"/>
-    <mergeCell ref="D11:D13"/>
-    <mergeCell ref="C11:C13"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="B6:D6"/>
-    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="J35:J42"/>
+    <mergeCell ref="D35:D36"/>
+    <mergeCell ref="C35:C36"/>
+    <mergeCell ref="D38:D40"/>
+    <mergeCell ref="C38:C40"/>
     <mergeCell ref="B38:B40"/>
     <mergeCell ref="A35:A42"/>
     <mergeCell ref="B35:B37"/>
@@ -2057,11 +2055,13 @@
     <mergeCell ref="B16:B34"/>
     <mergeCell ref="A9:A34"/>
     <mergeCell ref="B9:B15"/>
-    <mergeCell ref="J35:J42"/>
-    <mergeCell ref="D35:D36"/>
-    <mergeCell ref="C35:C36"/>
-    <mergeCell ref="D38:D40"/>
-    <mergeCell ref="C38:C40"/>
+    <mergeCell ref="A1:I1"/>
+    <mergeCell ref="D11:D13"/>
+    <mergeCell ref="C11:C13"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="B6:D6"/>
+    <mergeCell ref="E6:F6"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <drawing r:id="rId1"/>

</xml_diff>